<commit_message>
2019-08-19 : some bug fixed, reseting adjustments while re-import attendance - fixed
</commit_message>
<xml_diff>
--- a/ContractPayroll/BulkUploadFormat/Bulk_BasicChange.xlsx
+++ b/ContractPayroll/BulkUploadFormat/Bulk_BasicChange.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>40055106</v>
@@ -421,293 +421,33 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>43126</v>
+        <v>43550</v>
       </c>
       <c r="E2" s="1">
-        <v>43131</v>
+        <v>43555</v>
       </c>
       <c r="F2">
-        <v>500</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>40055111</v>
+        <v>40055106</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
-        <v>43126</v>
+        <v>43556</v>
       </c>
       <c r="E3" s="1">
-        <v>43131</v>
+        <v>43580</v>
       </c>
       <c r="F3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>40055112</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E4" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>40055114</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E5" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>40055116</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E6" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>40055120</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E7" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>40055126</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E8" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>40055157</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E9" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F9">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>40055199</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E10" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F10">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>40055268</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E11" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F11">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>40055373</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E12" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F12">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>40055429</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E13" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>40055436</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E14" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F14">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>40055616</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E15" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F15">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>40055755</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>43125</v>
-      </c>
-      <c r="E16" s="1">
-        <v>43131</v>
-      </c>
-      <c r="F16">
-        <v>500</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>